<commit_message>
Use Clang 14 as baseline in plots
</commit_message>
<xml_diff>
--- a/data/git/file/git.o.xlsx
+++ b/data/git/file/git.o.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jryans/Research/Papers/oopsla-2023/data/git/file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4EE94F-1886-AC42-99FA-F241CAEFF560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3B8E25-D8A3-F845-B160-26E10E7F6B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16440" yWindow="1920" windowWidth="47060" windowHeight="24880" activeTab="2" xr2:uid="{1069CAA2-7C27-E54E-B88A-C9343E41429C}"/>
+    <workbookView xWindow="16440" yWindow="1920" windowWidth="47060" windowHeight="24880" activeTab="1" xr2:uid="{1069CAA2-7C27-E54E-B88A-C9343E41429C}"/>
   </bookViews>
   <sheets>
     <sheet name="Wide" sheetId="1" r:id="rId1"/>
@@ -658,9 +658,6 @@
     <t>O1-14 Delta</t>
   </si>
   <si>
-    <t xml:space="preserve">CL / SL (O0-13, m2r)    </t>
-  </si>
-  <si>
     <t>CL / SL (O1-12)</t>
   </si>
   <si>
@@ -673,9 +670,6 @@
     <t>CL / SL Delta</t>
   </si>
   <si>
-    <t>CL (O0-13, m2r)</t>
-  </si>
-  <si>
     <t>CL (O1-12)</t>
   </si>
   <si>
@@ -683,24 +677,6 @@
   </si>
   <si>
     <t>CL (O1-14)</t>
-  </si>
-  <si>
-    <t>CL / SL (O0-13)</t>
-  </si>
-  <si>
-    <t>CL (O0-13)</t>
-  </si>
-  <si>
-    <t>Clang 13, O0</t>
-  </si>
-  <si>
-    <t>O0-13 Delta</t>
-  </si>
-  <si>
-    <t>O0-13, m2r Delta</t>
-  </si>
-  <si>
-    <t>Clang 13, O0 + mem2reg</t>
   </si>
   <si>
     <t>Arithmetic Mean (Normalised)</t>
@@ -717,14 +693,45 @@
   <si>
     <t>Clang 14, O2</t>
   </si>
+  <si>
+    <t>CL / SL (O0-14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL / SL (O0-14, m2r)    </t>
+  </si>
+  <si>
+    <t>O0-14 Delta</t>
+  </si>
+  <si>
+    <t>O0-14, m2r Delta</t>
+  </si>
+  <si>
+    <t>CL (O0-14)</t>
+  </si>
+  <si>
+    <t>CL (O0-14, m2r)</t>
+  </si>
+  <si>
+    <t>Clang 14, O0</t>
+  </si>
+  <si>
+    <t>Clang 14, O0 + mem2reg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -814,10 +821,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -853,59 +861,59 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_6" connectionId="17" xr16:uid="{BF097535-9BC4-8A44-8028-889020E90CD1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_4" connectionId="15" xr16:uid="{12472C14-9457-0C4B-85A7-6B4E9A0A4A3A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_3" connectionId="14" xr16:uid="{ED71FF77-6ABC-D749-8E21-C2BBC0C49B38}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_2" connectionId="13" xr16:uid="{577EB844-CFFF-874E-B636-A682F7CA9C09}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_10" connectionId="12" xr16:uid="{6F5AE438-0047-EF40-9065-31B57EBCFEA0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_9" connectionId="20" xr16:uid="{DF99720B-8FB8-1945-B82B-62174EC5794B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_9" connectionId="20" xr16:uid="{DF99720B-8FB8-1945-B82B-62174EC5794B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O013m2r" connectionId="2" xr16:uid="{9CCAF8A0-2B7D-0548-BCF8-D231422B6B5F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O113" connectionId="7" xr16:uid="{7EC8FDAA-8641-7F44-A40C-DFADA06143DC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O114" connectionId="9" xr16:uid="{6DA84D36-F075-D643-87AE-9205D8C2E13B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O013m2r" connectionId="3" xr16:uid="{6BD7D553-8716-684F-A112-947029E7B50E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O112" connectionId="5" xr16:uid="{5C22DE01-5C44-7C4E-9EAF-E54F03689DF7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O113" connectionId="7" xr16:uid="{7EC8FDAA-8641-7F44-A40C-DFADA06143DC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O112" connectionId="6" xr16:uid="{72FE5272-0C81-7B49-8C92-9E8FE63CCD65}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O114" connectionId="9" xr16:uid="{6DA84D36-F075-D643-87AE-9205D8C2E13B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O013m2r" connectionId="4" xr16:uid="{F1095D83-ED7E-9549-9DFC-EB98E00E3997}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O013m2r" connectionId="3" xr16:uid="{6BD7D553-8716-684F-A112-947029E7B50E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O114" connectionId="10" xr16:uid="{D34FF5A8-62F7-554D-9E92-8F5C8D099217}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_5" connectionId="16" xr16:uid="{5AF1A4D8-20C7-B944-973B-C6F106978454}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O113" connectionId="8" xr16:uid="{061FB766-530C-7F46-AA03-8A3221BEEC32}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O112" connectionId="6" xr16:uid="{72FE5272-0C81-7B49-8C92-9E8FE63CCD65}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O013m2r" connectionId="4" xr16:uid="{F1095D83-ED7E-9549-9DFC-EB98E00E3997}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_2" connectionId="13" xr16:uid="{577EB844-CFFF-874E-B636-A682F7CA9C09}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O114" connectionId="10" xr16:uid="{D34FF5A8-62F7-554D-9E92-8F5C8D099217}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_4" connectionId="15" xr16:uid="{12472C14-9457-0C4B-85A7-6B4E9A0A4A3A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_7" connectionId="18" xr16:uid="{D6E8256A-0710-A34A-80B4-71635A8A7FF9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -913,23 +921,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_3" connectionId="14" xr16:uid="{ED71FF77-6ABC-D749-8E21-C2BBC0C49B38}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_1" connectionId="11" xr16:uid="{3FDFE62B-64A1-F14C-AAB6-88B8E3E9B697}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_10" connectionId="12" xr16:uid="{6F5AE438-0047-EF40-9065-31B57EBCFEA0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_8" connectionId="19" xr16:uid="{6528BD19-FD94-5B40-8D88-624F75163B95}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o.O013m2r" connectionId="2" xr16:uid="{9CCAF8A0-2B7D-0548-BCF8-D231422B6B5F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_5" connectionId="16" xr16:uid="{5AF1A4D8-20C7-B944-973B-C6F106978454}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_7" connectionId="18" xr16:uid="{D6E8256A-0710-A34A-80B4-71635A8A7FF9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="git.o_6" connectionId="17" xr16:uid="{BF097535-9BC4-8A44-8028-889020E90CD1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1232,7 +1240,7 @@
   <dimension ref="A1:T101"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1260,31 +1268,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>106</v>
@@ -1296,19 +1304,19 @@
         <v>108</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -7426,8 +7434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E642B73-D860-1940-91EE-067F16E263DB}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -7443,15 +7451,15 @@
         <v>102</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>120</v>
+      <c r="A2" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="B2" s="7">
         <f>1+AVERAGE(Wide!J2:J101)</f>
@@ -7467,8 +7475,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>123</v>
+      <c r="A3" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="B3" s="7">
         <f>1+AVERAGE(Wide!K2:K101)</f>
@@ -7535,7 +7543,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7544,8 +7552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B95AD34-2DCB-AC43-B218-83D6A66E9916}">
   <dimension ref="A1:C601"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A574" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E596" sqref="E596"/>
+    <sheetView topLeftCell="A574" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J606" sqref="J606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -7572,7 +7580,7 @@
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>29</v>
@@ -7584,7 +7592,7 @@
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>83</v>
@@ -7596,7 +7604,7 @@
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>84</v>
@@ -7608,7 +7616,7 @@
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>85</v>
@@ -7620,7 +7628,7 @@
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>86</v>
@@ -7632,7 +7640,7 @@
     </row>
     <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>87</v>
@@ -7644,7 +7652,7 @@
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>88</v>
@@ -7656,7 +7664,7 @@
     </row>
     <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>25</v>
@@ -7668,7 +7676,7 @@
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>27</v>
@@ -7680,7 +7688,7 @@
     </row>
     <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>28</v>
@@ -7692,7 +7700,7 @@
     </row>
     <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>26</v>
@@ -7704,7 +7712,7 @@
     </row>
     <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>36</v>
@@ -7716,7 +7724,7 @@
     </row>
     <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>35</v>
@@ -7728,7 +7736,7 @@
     </row>
     <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>5</v>
@@ -7740,7 +7748,7 @@
     </row>
     <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>6</v>
@@ -7752,7 +7760,7 @@
     </row>
     <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
@@ -7764,7 +7772,7 @@
     </row>
     <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>31</v>
@@ -7776,7 +7784,7 @@
     </row>
     <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>32</v>
@@ -7788,7 +7796,7 @@
     </row>
     <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>30</v>
@@ -7800,7 +7808,7 @@
     </row>
     <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>100</v>
@@ -7812,7 +7820,7 @@
     </row>
     <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>67</v>
@@ -7824,7 +7832,7 @@
     </row>
     <row r="23" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>66</v>
@@ -7836,7 +7844,7 @@
     </row>
     <row r="24" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>78</v>
@@ -7848,7 +7856,7 @@
     </row>
     <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>79</v>
@@ -7860,7 +7868,7 @@
     </row>
     <row r="26" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>71</v>
@@ -7872,7 +7880,7 @@
     </row>
     <row r="27" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>72</v>
@@ -7884,7 +7892,7 @@
     </row>
     <row r="28" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>81</v>
@@ -7896,7 +7904,7 @@
     </row>
     <row r="29" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>74</v>
@@ -7908,7 +7916,7 @@
     </row>
     <row r="30" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>73</v>
@@ -7920,7 +7928,7 @@
     </row>
     <row r="31" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>75</v>
@@ -7932,7 +7940,7 @@
     </row>
     <row r="32" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>82</v>
@@ -7944,7 +7952,7 @@
     </row>
     <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>80</v>
@@ -7956,7 +7964,7 @@
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>76</v>
@@ -7968,7 +7976,7 @@
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>77</v>
@@ -7980,7 +7988,7 @@
     </row>
     <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>15</v>
@@ -7992,7 +8000,7 @@
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>17</v>
@@ -8004,7 +8012,7 @@
     </row>
     <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>16</v>
@@ -8016,7 +8024,7 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>19</v>
@@ -8028,7 +8036,7 @@
     </row>
     <row r="40" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>18</v>
@@ -8040,7 +8048,7 @@
     </row>
     <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>20</v>
@@ -8052,7 +8060,7 @@
     </row>
     <row r="42" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>90</v>
@@ -8064,7 +8072,7 @@
     </row>
     <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>89</v>
@@ -8076,7 +8084,7 @@
     </row>
     <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>93</v>
@@ -8088,7 +8096,7 @@
     </row>
     <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>94</v>
@@ -8100,7 +8108,7 @@
     </row>
     <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>91</v>
@@ -8112,7 +8120,7 @@
     </row>
     <row r="47" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>96</v>
@@ -8124,7 +8132,7 @@
     </row>
     <row r="48" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>95</v>
@@ -8136,7 +8144,7 @@
     </row>
     <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>92</v>
@@ -8148,7 +8156,7 @@
     </row>
     <row r="50" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>99</v>
@@ -8160,7 +8168,7 @@
     </row>
     <row r="51" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>64</v>
@@ -8172,7 +8180,7 @@
     </row>
     <row r="52" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>65</v>
@@ -8184,7 +8192,7 @@
     </row>
     <row r="53" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>63</v>
@@ -8196,7 +8204,7 @@
     </row>
     <row r="54" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>11</v>
@@ -8208,7 +8216,7 @@
     </row>
     <row r="55" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>13</v>
@@ -8220,7 +8228,7 @@
     </row>
     <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>9</v>
@@ -8232,7 +8240,7 @@
     </row>
     <row r="57" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>10</v>
@@ -8244,7 +8252,7 @@
     </row>
     <row r="58" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>14</v>
@@ -8256,7 +8264,7 @@
     </row>
     <row r="59" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>12</v>
@@ -8268,7 +8276,7 @@
     </row>
     <row r="60" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>8</v>
@@ -8280,7 +8288,7 @@
     </row>
     <row r="61" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>60</v>
@@ -8292,7 +8300,7 @@
     </row>
     <row r="62" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>62</v>
@@ -8304,7 +8312,7 @@
     </row>
     <row r="63" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>61</v>
@@ -8316,7 +8324,7 @@
     </row>
     <row r="64" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>59</v>
@@ -8328,7 +8336,7 @@
     </row>
     <row r="65" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>2</v>
@@ -8340,7 +8348,7 @@
     </row>
     <row r="66" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>1</v>
@@ -8352,7 +8360,7 @@
     </row>
     <row r="67" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>3</v>
@@ -8364,7 +8372,7 @@
     </row>
     <row r="68" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>4</v>
@@ -8376,7 +8384,7 @@
     </row>
     <row r="69" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>21</v>
@@ -8388,7 +8396,7 @@
     </row>
     <row r="70" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>23</v>
@@ -8400,7 +8408,7 @@
     </row>
     <row r="71" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>24</v>
@@ -8412,7 +8420,7 @@
     </row>
     <row r="72" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>22</v>
@@ -8424,7 +8432,7 @@
     </row>
     <row r="73" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>40</v>
@@ -8436,7 +8444,7 @@
     </row>
     <row r="74" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>41</v>
@@ -8448,7 +8456,7 @@
     </row>
     <row r="75" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>45</v>
@@ -8460,7 +8468,7 @@
     </row>
     <row r="76" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>42</v>
@@ -8472,7 +8480,7 @@
     </row>
     <row r="77" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>43</v>
@@ -8484,7 +8492,7 @@
     </row>
     <row r="78" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>46</v>
@@ -8496,7 +8504,7 @@
     </row>
     <row r="79" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>48</v>
@@ -8508,7 +8516,7 @@
     </row>
     <row r="80" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>49</v>
@@ -8520,7 +8528,7 @@
     </row>
     <row r="81" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>47</v>
@@ -8532,7 +8540,7 @@
     </row>
     <row r="82" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>44</v>
@@ -8544,7 +8552,7 @@
     </row>
     <row r="83" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>51</v>
@@ -8556,7 +8564,7 @@
     </row>
     <row r="84" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>52</v>
@@ -8568,7 +8576,7 @@
     </row>
     <row r="85" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>55</v>
@@ -8580,7 +8588,7 @@
     </row>
     <row r="86" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>58</v>
@@ -8592,7 +8600,7 @@
     </row>
     <row r="87" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>50</v>
@@ -8604,7 +8612,7 @@
     </row>
     <row r="88" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>56</v>
@@ -8616,7 +8624,7 @@
     </row>
     <row r="89" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>54</v>
@@ -8628,7 +8636,7 @@
     </row>
     <row r="90" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>53</v>
@@ -8640,7 +8648,7 @@
     </row>
     <row r="91" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>57</v>
@@ -8652,7 +8660,7 @@
     </row>
     <row r="92" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>33</v>
@@ -8664,7 +8672,7 @@
     </row>
     <row r="93" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>34</v>
@@ -8676,7 +8684,7 @@
     </row>
     <row r="94" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>70</v>
@@ -8688,7 +8696,7 @@
     </row>
     <row r="95" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>69</v>
@@ -8700,7 +8708,7 @@
     </row>
     <row r="96" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>68</v>
@@ -8712,7 +8720,7 @@
     </row>
     <row r="97" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>37</v>
@@ -8724,7 +8732,7 @@
     </row>
     <row r="98" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>38</v>
@@ -8736,7 +8744,7 @@
     </row>
     <row r="99" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>98</v>
@@ -8748,7 +8756,7 @@
     </row>
     <row r="100" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>97</v>
@@ -8760,7 +8768,7 @@
     </row>
     <row r="101" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>39</v>
@@ -8772,7 +8780,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>29</v>
@@ -8784,7 +8792,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>83</v>
@@ -8796,7 +8804,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>84</v>
@@ -8808,7 +8816,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>85</v>
@@ -8820,7 +8828,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>86</v>
@@ -8832,7 +8840,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>87</v>
@@ -8844,7 +8852,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>88</v>
@@ -8856,7 +8864,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>25</v>
@@ -8868,7 +8876,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>27</v>
@@ -8880,7 +8888,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>28</v>
@@ -8892,7 +8900,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>26</v>
@@ -8904,7 +8912,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>36</v>
@@ -8916,7 +8924,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>35</v>
@@ -8928,7 +8936,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>5</v>
@@ -8940,7 +8948,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>6</v>
@@ -8952,7 +8960,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>7</v>
@@ -8964,7 +8972,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>31</v>
@@ -8976,7 +8984,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>32</v>
@@ -8988,7 +8996,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>30</v>
@@ -9000,7 +9008,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>100</v>
@@ -9012,7 +9020,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>67</v>
@@ -9024,7 +9032,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>66</v>
@@ -9036,7 +9044,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>78</v>
@@ -9048,7 +9056,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>79</v>
@@ -9060,7 +9068,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>71</v>
@@ -9072,7 +9080,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>72</v>
@@ -9084,7 +9092,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>81</v>
@@ -9096,7 +9104,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>74</v>
@@ -9108,7 +9116,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>73</v>
@@ -9120,7 +9128,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>75</v>
@@ -9132,7 +9140,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>82</v>
@@ -9144,7 +9152,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>80</v>
@@ -9156,7 +9164,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>76</v>
@@ -9168,7 +9176,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>77</v>
@@ -9180,7 +9188,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>15</v>
@@ -9192,7 +9200,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>17</v>
@@ -9204,7 +9212,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>16</v>
@@ -9216,7 +9224,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>19</v>
@@ -9228,7 +9236,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>18</v>
@@ -9240,7 +9248,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>20</v>
@@ -9252,7 +9260,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>90</v>
@@ -9264,7 +9272,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>89</v>
@@ -9276,7 +9284,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>93</v>
@@ -9288,7 +9296,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>94</v>
@@ -9300,7 +9308,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>91</v>
@@ -9312,7 +9320,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>96</v>
@@ -9324,7 +9332,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>95</v>
@@ -9336,7 +9344,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>92</v>
@@ -9348,7 +9356,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>99</v>
@@ -9360,7 +9368,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>64</v>
@@ -9372,7 +9380,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>65</v>
@@ -9384,7 +9392,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>63</v>
@@ -9396,7 +9404,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>11</v>
@@ -9408,7 +9416,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>13</v>
@@ -9420,7 +9428,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>9</v>
@@ -9432,7 +9440,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>10</v>
@@ -9444,7 +9452,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>14</v>
@@ -9456,7 +9464,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>12</v>
@@ -9468,7 +9476,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>8</v>
@@ -9480,7 +9488,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>60</v>
@@ -9492,7 +9500,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>62</v>
@@ -9504,7 +9512,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>61</v>
@@ -9516,7 +9524,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>59</v>
@@ -9528,7 +9536,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>2</v>
@@ -9540,7 +9548,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>1</v>
@@ -9552,7 +9560,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>3</v>
@@ -9564,7 +9572,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>4</v>
@@ -9576,7 +9584,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>21</v>
@@ -9588,7 +9596,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>23</v>
@@ -9600,7 +9608,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>24</v>
@@ -9612,7 +9620,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>22</v>
@@ -9624,7 +9632,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>40</v>
@@ -9636,7 +9644,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>41</v>
@@ -9648,7 +9656,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>45</v>
@@ -9660,7 +9668,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>42</v>
@@ -9672,7 +9680,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>43</v>
@@ -9684,7 +9692,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>46</v>
@@ -9696,7 +9704,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>48</v>
@@ -9708,7 +9716,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>49</v>
@@ -9720,7 +9728,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>47</v>
@@ -9732,7 +9740,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>44</v>
@@ -9744,7 +9752,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>51</v>
@@ -9756,7 +9764,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>52</v>
@@ -9768,7 +9776,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>55</v>
@@ -9780,7 +9788,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>58</v>
@@ -9792,7 +9800,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>50</v>
@@ -9804,7 +9812,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>56</v>
@@ -9816,7 +9824,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>54</v>
@@ -9828,7 +9836,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>53</v>
@@ -9840,7 +9848,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>57</v>
@@ -9852,7 +9860,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>33</v>
@@ -9864,7 +9872,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B193" s="3" t="s">
         <v>34</v>
@@ -9876,7 +9884,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B194" s="3" t="s">
         <v>70</v>
@@ -9888,7 +9896,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B195" s="3" t="s">
         <v>69</v>
@@ -9900,7 +9908,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>68</v>
@@ -9912,7 +9920,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>37</v>
@@ -9924,7 +9932,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>38</v>
@@ -9936,7 +9944,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B199" s="3" t="s">
         <v>98</v>
@@ -9948,7 +9956,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>97</v>
@@ -9960,7 +9968,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>39</v>
@@ -13572,7 +13580,7 @@
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A502" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B502" s="3" t="s">
         <v>29</v>
@@ -13584,7 +13592,7 @@
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A503" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B503" s="3" t="s">
         <v>83</v>
@@ -13596,7 +13604,7 @@
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A504" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B504" s="3" t="s">
         <v>84</v>
@@ -13608,7 +13616,7 @@
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A505" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B505" s="3" t="s">
         <v>85</v>
@@ -13620,7 +13628,7 @@
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A506" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B506" s="3" t="s">
         <v>86</v>
@@ -13632,7 +13640,7 @@
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A507" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B507" s="3" t="s">
         <v>87</v>
@@ -13644,7 +13652,7 @@
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A508" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B508" s="3" t="s">
         <v>88</v>
@@ -13656,7 +13664,7 @@
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A509" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B509" s="3" t="s">
         <v>25</v>
@@ -13668,7 +13676,7 @@
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A510" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B510" s="3" t="s">
         <v>27</v>
@@ -13680,7 +13688,7 @@
     </row>
     <row r="511" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A511" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B511" s="3" t="s">
         <v>28</v>
@@ -13692,7 +13700,7 @@
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A512" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B512" s="3" t="s">
         <v>26</v>
@@ -13704,7 +13712,7 @@
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A513" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B513" s="3" t="s">
         <v>36</v>
@@ -13716,7 +13724,7 @@
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A514" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B514" s="3" t="s">
         <v>35</v>
@@ -13728,7 +13736,7 @@
     </row>
     <row r="515" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A515" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B515" s="3" t="s">
         <v>5</v>
@@ -13740,7 +13748,7 @@
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A516" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B516" s="3" t="s">
         <v>6</v>
@@ -13752,7 +13760,7 @@
     </row>
     <row r="517" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A517" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B517" s="3" t="s">
         <v>7</v>
@@ -13764,7 +13772,7 @@
     </row>
     <row r="518" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A518" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B518" s="3" t="s">
         <v>31</v>
@@ -13776,7 +13784,7 @@
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A519" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B519" s="3" t="s">
         <v>32</v>
@@ -13788,7 +13796,7 @@
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A520" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B520" s="3" t="s">
         <v>30</v>
@@ -13800,7 +13808,7 @@
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A521" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B521" s="3" t="s">
         <v>100</v>
@@ -13812,7 +13820,7 @@
     </row>
     <row r="522" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A522" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B522" s="3" t="s">
         <v>67</v>
@@ -13824,7 +13832,7 @@
     </row>
     <row r="523" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A523" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B523" s="3" t="s">
         <v>66</v>
@@ -13836,7 +13844,7 @@
     </row>
     <row r="524" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A524" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B524" s="3" t="s">
         <v>78</v>
@@ -13848,7 +13856,7 @@
     </row>
     <row r="525" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A525" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B525" s="3" t="s">
         <v>79</v>
@@ -13860,7 +13868,7 @@
     </row>
     <row r="526" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A526" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B526" s="3" t="s">
         <v>71</v>
@@ -13872,7 +13880,7 @@
     </row>
     <row r="527" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A527" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B527" s="3" t="s">
         <v>72</v>
@@ -13884,7 +13892,7 @@
     </row>
     <row r="528" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A528" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B528" s="3" t="s">
         <v>81</v>
@@ -13896,7 +13904,7 @@
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A529" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B529" s="3" t="s">
         <v>74</v>
@@ -13908,7 +13916,7 @@
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A530" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B530" s="3" t="s">
         <v>73</v>
@@ -13920,7 +13928,7 @@
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A531" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B531" s="3" t="s">
         <v>75</v>
@@ -13932,7 +13940,7 @@
     </row>
     <row r="532" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A532" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B532" s="3" t="s">
         <v>82</v>
@@ -13944,7 +13952,7 @@
     </row>
     <row r="533" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A533" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B533" s="3" t="s">
         <v>80</v>
@@ -13956,7 +13964,7 @@
     </row>
     <row r="534" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A534" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B534" s="3" t="s">
         <v>76</v>
@@ -13968,7 +13976,7 @@
     </row>
     <row r="535" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A535" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B535" s="3" t="s">
         <v>77</v>
@@ -13980,7 +13988,7 @@
     </row>
     <row r="536" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A536" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B536" s="3" t="s">
         <v>15</v>
@@ -13992,7 +14000,7 @@
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A537" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B537" s="3" t="s">
         <v>17</v>
@@ -14004,7 +14012,7 @@
     </row>
     <row r="538" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A538" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B538" s="3" t="s">
         <v>16</v>
@@ -14016,7 +14024,7 @@
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A539" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B539" s="3" t="s">
         <v>19</v>
@@ -14028,7 +14036,7 @@
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A540" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B540" s="3" t="s">
         <v>18</v>
@@ -14040,7 +14048,7 @@
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A541" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B541" s="3" t="s">
         <v>20</v>
@@ -14052,7 +14060,7 @@
     </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A542" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B542" s="3" t="s">
         <v>90</v>
@@ -14064,7 +14072,7 @@
     </row>
     <row r="543" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A543" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B543" s="3" t="s">
         <v>89</v>
@@ -14076,7 +14084,7 @@
     </row>
     <row r="544" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A544" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B544" s="3" t="s">
         <v>93</v>
@@ -14088,7 +14096,7 @@
     </row>
     <row r="545" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A545" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B545" s="3" t="s">
         <v>94</v>
@@ -14100,7 +14108,7 @@
     </row>
     <row r="546" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A546" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B546" s="3" t="s">
         <v>91</v>
@@ -14112,7 +14120,7 @@
     </row>
     <row r="547" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A547" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B547" s="3" t="s">
         <v>96</v>
@@ -14124,7 +14132,7 @@
     </row>
     <row r="548" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A548" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B548" s="3" t="s">
         <v>95</v>
@@ -14136,7 +14144,7 @@
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A549" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B549" s="3" t="s">
         <v>92</v>
@@ -14148,7 +14156,7 @@
     </row>
     <row r="550" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A550" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B550" s="3" t="s">
         <v>99</v>
@@ -14160,7 +14168,7 @@
     </row>
     <row r="551" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A551" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B551" s="3" t="s">
         <v>64</v>
@@ -14172,7 +14180,7 @@
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A552" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B552" s="3" t="s">
         <v>65</v>
@@ -14184,7 +14192,7 @@
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A553" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B553" s="3" t="s">
         <v>63</v>
@@ -14196,7 +14204,7 @@
     </row>
     <row r="554" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A554" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B554" s="3" t="s">
         <v>11</v>
@@ -14208,7 +14216,7 @@
     </row>
     <row r="555" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A555" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B555" s="3" t="s">
         <v>13</v>
@@ -14220,7 +14228,7 @@
     </row>
     <row r="556" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A556" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B556" s="3" t="s">
         <v>9</v>
@@ -14232,7 +14240,7 @@
     </row>
     <row r="557" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A557" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B557" s="3" t="s">
         <v>10</v>
@@ -14244,7 +14252,7 @@
     </row>
     <row r="558" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A558" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B558" s="3" t="s">
         <v>14</v>
@@ -14256,7 +14264,7 @@
     </row>
     <row r="559" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A559" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B559" s="3" t="s">
         <v>12</v>
@@ -14268,7 +14276,7 @@
     </row>
     <row r="560" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A560" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B560" s="3" t="s">
         <v>8</v>
@@ -14280,7 +14288,7 @@
     </row>
     <row r="561" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A561" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B561" s="3" t="s">
         <v>60</v>
@@ -14292,7 +14300,7 @@
     </row>
     <row r="562" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A562" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B562" s="3" t="s">
         <v>62</v>
@@ -14304,7 +14312,7 @@
     </row>
     <row r="563" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A563" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B563" s="3" t="s">
         <v>61</v>
@@ -14316,7 +14324,7 @@
     </row>
     <row r="564" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A564" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B564" s="3" t="s">
         <v>59</v>
@@ -14328,7 +14336,7 @@
     </row>
     <row r="565" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A565" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B565" s="3" t="s">
         <v>2</v>
@@ -14340,7 +14348,7 @@
     </row>
     <row r="566" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A566" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B566" s="3" t="s">
         <v>1</v>
@@ -14352,7 +14360,7 @@
     </row>
     <row r="567" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A567" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B567" s="3" t="s">
         <v>3</v>
@@ -14364,7 +14372,7 @@
     </row>
     <row r="568" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A568" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B568" s="3" t="s">
         <v>4</v>
@@ -14376,7 +14384,7 @@
     </row>
     <row r="569" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A569" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B569" s="3" t="s">
         <v>21</v>
@@ -14388,7 +14396,7 @@
     </row>
     <row r="570" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A570" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B570" s="3" t="s">
         <v>23</v>
@@ -14400,7 +14408,7 @@
     </row>
     <row r="571" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A571" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B571" s="3" t="s">
         <v>24</v>
@@ -14412,7 +14420,7 @@
     </row>
     <row r="572" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A572" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B572" s="3" t="s">
         <v>22</v>
@@ -14424,7 +14432,7 @@
     </row>
     <row r="573" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A573" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B573" s="3" t="s">
         <v>40</v>
@@ -14436,7 +14444,7 @@
     </row>
     <row r="574" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A574" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B574" s="3" t="s">
         <v>41</v>
@@ -14448,7 +14456,7 @@
     </row>
     <row r="575" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A575" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B575" s="3" t="s">
         <v>45</v>
@@ -14460,7 +14468,7 @@
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A576" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B576" s="3" t="s">
         <v>42</v>
@@ -14472,7 +14480,7 @@
     </row>
     <row r="577" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A577" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B577" s="3" t="s">
         <v>43</v>
@@ -14484,7 +14492,7 @@
     </row>
     <row r="578" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A578" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B578" s="3" t="s">
         <v>46</v>
@@ -14496,7 +14504,7 @@
     </row>
     <row r="579" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A579" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B579" s="3" t="s">
         <v>48</v>
@@ -14508,7 +14516,7 @@
     </row>
     <row r="580" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A580" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B580" s="3" t="s">
         <v>49</v>
@@ -14520,7 +14528,7 @@
     </row>
     <row r="581" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A581" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B581" s="3" t="s">
         <v>47</v>
@@ -14532,7 +14540,7 @@
     </row>
     <row r="582" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A582" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B582" s="3" t="s">
         <v>44</v>
@@ -14544,7 +14552,7 @@
     </row>
     <row r="583" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A583" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B583" s="3" t="s">
         <v>51</v>
@@ -14556,7 +14564,7 @@
     </row>
     <row r="584" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A584" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B584" s="3" t="s">
         <v>52</v>
@@ -14568,7 +14576,7 @@
     </row>
     <row r="585" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A585" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B585" s="3" t="s">
         <v>55</v>
@@ -14580,7 +14588,7 @@
     </row>
     <row r="586" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A586" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B586" s="3" t="s">
         <v>58</v>
@@ -14592,7 +14600,7 @@
     </row>
     <row r="587" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A587" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B587" s="3" t="s">
         <v>50</v>
@@ -14604,7 +14612,7 @@
     </row>
     <row r="588" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A588" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B588" s="3" t="s">
         <v>56</v>
@@ -14616,7 +14624,7 @@
     </row>
     <row r="589" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A589" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B589" s="3" t="s">
         <v>54</v>
@@ -14628,7 +14636,7 @@
     </row>
     <row r="590" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A590" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B590" s="3" t="s">
         <v>53</v>
@@ -14640,7 +14648,7 @@
     </row>
     <row r="591" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A591" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B591" s="3" t="s">
         <v>57</v>
@@ -14652,7 +14660,7 @@
     </row>
     <row r="592" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A592" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B592" s="3" t="s">
         <v>33</v>
@@ -14664,7 +14672,7 @@
     </row>
     <row r="593" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A593" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B593" s="3" t="s">
         <v>34</v>
@@ -14676,7 +14684,7 @@
     </row>
     <row r="594" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A594" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B594" s="3" t="s">
         <v>70</v>
@@ -14688,7 +14696,7 @@
     </row>
     <row r="595" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A595" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B595" s="3" t="s">
         <v>69</v>
@@ -14700,7 +14708,7 @@
     </row>
     <row r="596" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A596" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B596" s="3" t="s">
         <v>68</v>
@@ -14712,7 +14720,7 @@
     </row>
     <row r="597" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A597" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B597" s="3" t="s">
         <v>37</v>
@@ -14724,7 +14732,7 @@
     </row>
     <row r="598" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A598" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B598" s="3" t="s">
         <v>38</v>
@@ -14736,7 +14744,7 @@
     </row>
     <row r="599" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A599" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B599" s="3" t="s">
         <v>98</v>
@@ -14748,7 +14756,7 @@
     </row>
     <row r="600" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A600" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B600" s="3" t="s">
         <v>97</v>
@@ -14760,7 +14768,7 @@
     </row>
     <row r="601" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A601" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B601" s="3" t="s">
         <v>39</v>
@@ -14771,7 +14779,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14780,7 +14788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84346BFC-D007-624F-A0A1-2C793D8563B9}">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
@@ -14803,12 +14811,12 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>29</v>
@@ -14820,7 +14828,7 @@
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>83</v>
@@ -14832,7 +14840,7 @@
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>84</v>
@@ -14844,7 +14852,7 @@
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>85</v>
@@ -14856,7 +14864,7 @@
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>86</v>
@@ -14868,7 +14876,7 @@
     </row>
     <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>87</v>
@@ -14880,7 +14888,7 @@
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>88</v>
@@ -14892,7 +14900,7 @@
     </row>
     <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>25</v>
@@ -14904,7 +14912,7 @@
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>27</v>
@@ -14916,7 +14924,7 @@
     </row>
     <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>28</v>
@@ -14928,7 +14936,7 @@
     </row>
     <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
@@ -14940,7 +14948,7 @@
     </row>
     <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>36</v>
@@ -14952,7 +14960,7 @@
     </row>
     <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>35</v>
@@ -14964,7 +14972,7 @@
     </row>
     <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
@@ -14976,7 +14984,7 @@
     </row>
     <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -14988,7 +14996,7 @@
     </row>
     <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
@@ -15000,7 +15008,7 @@
     </row>
     <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>31</v>
@@ -15012,7 +15020,7 @@
     </row>
     <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>32</v>
@@ -15024,7 +15032,7 @@
     </row>
     <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>30</v>
@@ -15036,7 +15044,7 @@
     </row>
     <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>100</v>
@@ -15048,7 +15056,7 @@
     </row>
     <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>67</v>
@@ -15060,7 +15068,7 @@
     </row>
     <row r="23" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>66</v>
@@ -15072,7 +15080,7 @@
     </row>
     <row r="24" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>78</v>
@@ -15084,7 +15092,7 @@
     </row>
     <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>79</v>
@@ -15096,7 +15104,7 @@
     </row>
     <row r="26" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>71</v>
@@ -15108,7 +15116,7 @@
     </row>
     <row r="27" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>72</v>
@@ -15120,7 +15128,7 @@
     </row>
     <row r="28" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>81</v>
@@ -15132,7 +15140,7 @@
     </row>
     <row r="29" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>74</v>
@@ -15144,7 +15152,7 @@
     </row>
     <row r="30" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>73</v>
@@ -15156,7 +15164,7 @@
     </row>
     <row r="31" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>75</v>
@@ -15168,7 +15176,7 @@
     </row>
     <row r="32" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>82</v>
@@ -15180,7 +15188,7 @@
     </row>
     <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>80</v>
@@ -15192,7 +15200,7 @@
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>76</v>
@@ -15204,7 +15212,7 @@
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>77</v>
@@ -15216,7 +15224,7 @@
     </row>
     <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>15</v>
@@ -15228,7 +15236,7 @@
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>17</v>
@@ -15240,7 +15248,7 @@
     </row>
     <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>16</v>
@@ -15252,7 +15260,7 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>19</v>
@@ -15264,7 +15272,7 @@
     </row>
     <row r="40" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>18</v>
@@ -15276,7 +15284,7 @@
     </row>
     <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>20</v>
@@ -15288,7 +15296,7 @@
     </row>
     <row r="42" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>90</v>
@@ -15300,7 +15308,7 @@
     </row>
     <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>89</v>
@@ -15312,7 +15320,7 @@
     </row>
     <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>93</v>
@@ -15324,7 +15332,7 @@
     </row>
     <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>94</v>
@@ -15336,7 +15344,7 @@
     </row>
     <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>91</v>
@@ -15348,7 +15356,7 @@
     </row>
     <row r="47" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>96</v>
@@ -15360,7 +15368,7 @@
     </row>
     <row r="48" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>95</v>
@@ -15372,7 +15380,7 @@
     </row>
     <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>92</v>
@@ -15384,7 +15392,7 @@
     </row>
     <row r="50" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>99</v>
@@ -15396,7 +15404,7 @@
     </row>
     <row r="51" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>64</v>
@@ -15408,7 +15416,7 @@
     </row>
     <row r="52" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>65</v>
@@ -15420,7 +15428,7 @@
     </row>
     <row r="53" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>63</v>
@@ -15432,7 +15440,7 @@
     </row>
     <row r="54" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>11</v>
@@ -15444,7 +15452,7 @@
     </row>
     <row r="55" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>13</v>
@@ -15456,7 +15464,7 @@
     </row>
     <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>9</v>
@@ -15468,7 +15476,7 @@
     </row>
     <row r="57" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>10</v>
@@ -15480,7 +15488,7 @@
     </row>
     <row r="58" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>14</v>
@@ -15492,7 +15500,7 @@
     </row>
     <row r="59" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>12</v>
@@ -15504,7 +15512,7 @@
     </row>
     <row r="60" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>8</v>
@@ -15516,7 +15524,7 @@
     </row>
     <row r="61" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>60</v>
@@ -15528,7 +15536,7 @@
     </row>
     <row r="62" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>62</v>
@@ -15540,7 +15548,7 @@
     </row>
     <row r="63" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>61</v>
@@ -15552,7 +15560,7 @@
     </row>
     <row r="64" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>59</v>
@@ -15564,7 +15572,7 @@
     </row>
     <row r="65" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>2</v>
@@ -15576,7 +15584,7 @@
     </row>
     <row r="66" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>1</v>
@@ -15588,7 +15596,7 @@
     </row>
     <row r="67" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>3</v>
@@ -15600,7 +15608,7 @@
     </row>
     <row r="68" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>4</v>
@@ -15612,7 +15620,7 @@
     </row>
     <row r="69" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>21</v>
@@ -15624,7 +15632,7 @@
     </row>
     <row r="70" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>23</v>
@@ -15636,7 +15644,7 @@
     </row>
     <row r="71" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>24</v>
@@ -15648,7 +15656,7 @@
     </row>
     <row r="72" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>22</v>
@@ -15660,7 +15668,7 @@
     </row>
     <row r="73" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>40</v>
@@ -15672,7 +15680,7 @@
     </row>
     <row r="74" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>41</v>
@@ -15684,7 +15692,7 @@
     </row>
     <row r="75" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>45</v>
@@ -15696,7 +15704,7 @@
     </row>
     <row r="76" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>42</v>
@@ -15708,7 +15716,7 @@
     </row>
     <row r="77" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>43</v>
@@ -15720,7 +15728,7 @@
     </row>
     <row r="78" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>46</v>
@@ -15732,7 +15740,7 @@
     </row>
     <row r="79" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>48</v>
@@ -15744,7 +15752,7 @@
     </row>
     <row r="80" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>49</v>
@@ -15756,7 +15764,7 @@
     </row>
     <row r="81" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>47</v>
@@ -15768,7 +15776,7 @@
     </row>
     <row r="82" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>44</v>
@@ -15780,7 +15788,7 @@
     </row>
     <row r="83" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>51</v>
@@ -15792,7 +15800,7 @@
     </row>
     <row r="84" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>52</v>
@@ -15804,7 +15812,7 @@
     </row>
     <row r="85" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>55</v>
@@ -15816,7 +15824,7 @@
     </row>
     <row r="86" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>58</v>
@@ -15828,7 +15836,7 @@
     </row>
     <row r="87" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>50</v>
@@ -15840,7 +15848,7 @@
     </row>
     <row r="88" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>56</v>
@@ -15852,7 +15860,7 @@
     </row>
     <row r="89" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>54</v>
@@ -15864,7 +15872,7 @@
     </row>
     <row r="90" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>53</v>
@@ -15876,7 +15884,7 @@
     </row>
     <row r="91" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>57</v>
@@ -15888,7 +15896,7 @@
     </row>
     <row r="92" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>33</v>
@@ -15900,7 +15908,7 @@
     </row>
     <row r="93" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>34</v>
@@ -15912,7 +15920,7 @@
     </row>
     <row r="94" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>70</v>
@@ -15924,7 +15932,7 @@
     </row>
     <row r="95" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>69</v>
@@ -15936,7 +15944,7 @@
     </row>
     <row r="96" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>68</v>
@@ -15948,7 +15956,7 @@
     </row>
     <row r="97" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>37</v>
@@ -15960,7 +15968,7 @@
     </row>
     <row r="98" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>38</v>
@@ -15972,7 +15980,7 @@
     </row>
     <row r="99" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>98</v>
@@ -15984,7 +15992,7 @@
     </row>
     <row r="100" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>97</v>
@@ -15996,7 +16004,7 @@
     </row>
     <row r="101" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>39</v>
@@ -16008,7 +16016,7 @@
     </row>
     <row r="102" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>29</v>
@@ -16020,7 +16028,7 @@
     </row>
     <row r="103" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>83</v>
@@ -16032,7 +16040,7 @@
     </row>
     <row r="104" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>84</v>
@@ -16044,7 +16052,7 @@
     </row>
     <row r="105" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>85</v>
@@ -16056,7 +16064,7 @@
     </row>
     <row r="106" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>86</v>
@@ -16068,7 +16076,7 @@
     </row>
     <row r="107" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>87</v>
@@ -16080,7 +16088,7 @@
     </row>
     <row r="108" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>88</v>
@@ -16092,7 +16100,7 @@
     </row>
     <row r="109" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>25</v>
@@ -16104,7 +16112,7 @@
     </row>
     <row r="110" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>27</v>
@@ -16116,7 +16124,7 @@
     </row>
     <row r="111" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>28</v>
@@ -16128,7 +16136,7 @@
     </row>
     <row r="112" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>26</v>
@@ -16140,7 +16148,7 @@
     </row>
     <row r="113" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>36</v>
@@ -16152,7 +16160,7 @@
     </row>
     <row r="114" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>35</v>
@@ -16164,7 +16172,7 @@
     </row>
     <row r="115" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>5</v>
@@ -16176,7 +16184,7 @@
     </row>
     <row r="116" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>6</v>
@@ -16188,7 +16196,7 @@
     </row>
     <row r="117" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>7</v>
@@ -16200,7 +16208,7 @@
     </row>
     <row r="118" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>31</v>
@@ -16212,7 +16220,7 @@
     </row>
     <row r="119" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>32</v>
@@ -16224,7 +16232,7 @@
     </row>
     <row r="120" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>30</v>
@@ -16236,7 +16244,7 @@
     </row>
     <row r="121" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>100</v>
@@ -16248,7 +16256,7 @@
     </row>
     <row r="122" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>67</v>
@@ -16260,7 +16268,7 @@
     </row>
     <row r="123" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>66</v>
@@ -16272,7 +16280,7 @@
     </row>
     <row r="124" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>78</v>
@@ -16284,7 +16292,7 @@
     </row>
     <row r="125" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>79</v>
@@ -16296,7 +16304,7 @@
     </row>
     <row r="126" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>71</v>
@@ -16308,7 +16316,7 @@
     </row>
     <row r="127" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>72</v>
@@ -16320,7 +16328,7 @@
     </row>
     <row r="128" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>81</v>
@@ -16332,7 +16340,7 @@
     </row>
     <row r="129" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>74</v>
@@ -16344,7 +16352,7 @@
     </row>
     <row r="130" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>73</v>
@@ -16356,7 +16364,7 @@
     </row>
     <row r="131" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>75</v>
@@ -16368,7 +16376,7 @@
     </row>
     <row r="132" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>82</v>
@@ -16380,7 +16388,7 @@
     </row>
     <row r="133" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>80</v>
@@ -16392,7 +16400,7 @@
     </row>
     <row r="134" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>76</v>
@@ -16404,7 +16412,7 @@
     </row>
     <row r="135" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>77</v>
@@ -16416,7 +16424,7 @@
     </row>
     <row r="136" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>15</v>
@@ -16428,7 +16436,7 @@
     </row>
     <row r="137" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>17</v>
@@ -16440,7 +16448,7 @@
     </row>
     <row r="138" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>16</v>
@@ -16452,7 +16460,7 @@
     </row>
     <row r="139" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>19</v>
@@ -16464,7 +16472,7 @@
     </row>
     <row r="140" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>18</v>
@@ -16476,7 +16484,7 @@
     </row>
     <row r="141" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>20</v>
@@ -16488,7 +16496,7 @@
     </row>
     <row r="142" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>90</v>
@@ -16500,7 +16508,7 @@
     </row>
     <row r="143" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>89</v>
@@ -16512,7 +16520,7 @@
     </row>
     <row r="144" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>93</v>
@@ -16524,7 +16532,7 @@
     </row>
     <row r="145" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>94</v>
@@ -16536,7 +16544,7 @@
     </row>
     <row r="146" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>91</v>
@@ -16548,7 +16556,7 @@
     </row>
     <row r="147" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>96</v>
@@ -16560,7 +16568,7 @@
     </row>
     <row r="148" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>95</v>
@@ -16572,7 +16580,7 @@
     </row>
     <row r="149" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>92</v>
@@ -16584,7 +16592,7 @@
     </row>
     <row r="150" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>99</v>
@@ -16596,7 +16604,7 @@
     </row>
     <row r="151" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>64</v>
@@ -16608,7 +16616,7 @@
     </row>
     <row r="152" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>65</v>
@@ -16620,7 +16628,7 @@
     </row>
     <row r="153" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>63</v>
@@ -16632,7 +16640,7 @@
     </row>
     <row r="154" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>11</v>
@@ -16644,7 +16652,7 @@
     </row>
     <row r="155" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>13</v>
@@ -16656,7 +16664,7 @@
     </row>
     <row r="156" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>9</v>
@@ -16668,7 +16676,7 @@
     </row>
     <row r="157" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>10</v>
@@ -16680,7 +16688,7 @@
     </row>
     <row r="158" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>14</v>
@@ -16692,7 +16700,7 @@
     </row>
     <row r="159" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>12</v>
@@ -16704,7 +16712,7 @@
     </row>
     <row r="160" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>8</v>
@@ -16716,7 +16724,7 @@
     </row>
     <row r="161" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>60</v>
@@ -16728,7 +16736,7 @@
     </row>
     <row r="162" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>62</v>
@@ -16740,7 +16748,7 @@
     </row>
     <row r="163" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>61</v>
@@ -16752,7 +16760,7 @@
     </row>
     <row r="164" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>59</v>
@@ -16764,7 +16772,7 @@
     </row>
     <row r="165" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>2</v>
@@ -16776,7 +16784,7 @@
     </row>
     <row r="166" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>1</v>
@@ -16788,7 +16796,7 @@
     </row>
     <row r="167" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>3</v>
@@ -16800,7 +16808,7 @@
     </row>
     <row r="168" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>4</v>
@@ -16812,7 +16820,7 @@
     </row>
     <row r="169" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>21</v>
@@ -16824,7 +16832,7 @@
     </row>
     <row r="170" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>23</v>
@@ -16836,7 +16844,7 @@
     </row>
     <row r="171" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>24</v>
@@ -16848,7 +16856,7 @@
     </row>
     <row r="172" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>22</v>
@@ -16860,7 +16868,7 @@
     </row>
     <row r="173" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>40</v>
@@ -16872,7 +16880,7 @@
     </row>
     <row r="174" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>41</v>
@@ -16884,7 +16892,7 @@
     </row>
     <row r="175" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>45</v>
@@ -16896,7 +16904,7 @@
     </row>
     <row r="176" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>42</v>
@@ -16908,7 +16916,7 @@
     </row>
     <row r="177" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>43</v>
@@ -16920,7 +16928,7 @@
     </row>
     <row r="178" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>46</v>
@@ -16932,7 +16940,7 @@
     </row>
     <row r="179" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>48</v>
@@ -16944,7 +16952,7 @@
     </row>
     <row r="180" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>49</v>
@@ -16956,7 +16964,7 @@
     </row>
     <row r="181" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>47</v>
@@ -16968,7 +16976,7 @@
     </row>
     <row r="182" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>44</v>
@@ -16980,7 +16988,7 @@
     </row>
     <row r="183" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>51</v>
@@ -16992,7 +17000,7 @@
     </row>
     <row r="184" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>52</v>
@@ -17004,7 +17012,7 @@
     </row>
     <row r="185" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>55</v>
@@ -17016,7 +17024,7 @@
     </row>
     <row r="186" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>58</v>
@@ -17028,7 +17036,7 @@
     </row>
     <row r="187" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>50</v>
@@ -17040,7 +17048,7 @@
     </row>
     <row r="188" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>56</v>
@@ -17052,7 +17060,7 @@
     </row>
     <row r="189" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>54</v>
@@ -17064,7 +17072,7 @@
     </row>
     <row r="190" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>53</v>
@@ -17076,7 +17084,7 @@
     </row>
     <row r="191" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>57</v>
@@ -17088,7 +17096,7 @@
     </row>
     <row r="192" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>33</v>
@@ -17100,7 +17108,7 @@
     </row>
     <row r="193" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>34</v>
@@ -17112,7 +17120,7 @@
     </row>
     <row r="194" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>70</v>
@@ -17124,7 +17132,7 @@
     </row>
     <row r="195" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>69</v>
@@ -17136,7 +17144,7 @@
     </row>
     <row r="196" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>68</v>
@@ -17148,7 +17156,7 @@
     </row>
     <row r="197" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>37</v>
@@ -17160,7 +17168,7 @@
     </row>
     <row r="198" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>38</v>
@@ -17172,7 +17180,7 @@
     </row>
     <row r="199" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>98</v>
@@ -17184,7 +17192,7 @@
     </row>
     <row r="200" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>97</v>
@@ -17196,7 +17204,7 @@
     </row>
     <row r="201" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>39</v>

</xml_diff>